<commit_message>
partial CMH/DH changes, TODO: Fix textbox output from spreadsheet
</commit_message>
<xml_diff>
--- a/bin/Debug/PowerSpreadSheet/PowerPrice.xlsx
+++ b/bin/Debug/PowerSpreadSheet/PowerPrice.xlsx
@@ -11,12 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
-  <si>
-    <t>DH &amp; 3H</t>
-  </si>
-  <si>
-    <t>CMH</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+  <si>
+    <t>Hashboard Settings</t>
   </si>
   <si>
     <t>Power Price ($/MW)</t>
@@ -25,34 +22,34 @@
     <t>16nm</t>
   </si>
   <si>
+    <t>14nm</t>
+  </si>
+  <si>
     <t>Clarke</t>
   </si>
   <si>
-    <t>14nm</t>
-  </si>
-  <si>
-    <t>&lt; 75</t>
+    <t>&lt; 30</t>
   </si>
   <si>
     <t>Full</t>
   </si>
   <si>
-    <t>75 - 90</t>
+    <t>32 - 53</t>
   </si>
   <si>
     <t>Eco</t>
   </si>
   <si>
-    <t>90 - 118</t>
-  </si>
-  <si>
-    <t>118 - 185</t>
+    <t>53 - 71</t>
+  </si>
+  <si>
+    <t>71 - 92</t>
   </si>
   <si>
     <t>Standby</t>
   </si>
   <si>
-    <t>&gt; 185</t>
+    <t>&gt; 92</t>
   </si>
 </sst>
 </file>
@@ -324,102 +321,99 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1">
-        <v>43691.0</v>
+        <v>43776.0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3">
-        <v>42.0</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>29.0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3">
-        <v>42.0</v>
+      <c r="C6" s="3">
+        <v>29.0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3">
-        <v>42.0</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <v>29.0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>